<commit_message>
Created maquette(design + prototype), all screens, wrote logic, which i will implement later,; created logic for back button, implemented it; made a routes for ecrans
Created maquette(design + prototype), all screens, wrote logic, which i will implement later,; created logic for back button, implemented it; made a routes for ecrans; rediraection from diferents ecrans; [IN TOTAL] made a good base of project, and implemented back logic. JDT
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC64A49-C729-4ED9-B44B-DBE3BCAE7634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46B6A86-603A-4638-AC02-029D29379C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="29625" yWindow="495" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Discussion, des taches du projet</t>
+  </si>
+  <si>
+    <t>Created maquette(design + prototype)</t>
+  </si>
+  <si>
+    <t>tous les écrans, j'ai écrit la logique, que j'implémenterai plus tard ; j'ai créé la logique pour le bouton retour, je l'ai implémentée ; j'ai fait des routes pour les écrans ; [AU TOTAL] j'ai fait une bonne base de projet et j'ai implémenté la logique retour.</t>
+  </si>
+  <si>
+    <t>JDT GitHub(Commits + release)</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1085,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1091,10 +1100,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13541666666666666</c:v>
+                  <c:v>0.17708333333333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2007,7 +2016,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2069,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 5 heurs 4 minutes</v>
+        <v>0 jours 7 heurs 40 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2075,15 +2084,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>305</v>
+        <v>460</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2316,15 +2325,21 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="46">
-        <v>45744</v>
-      </c>
-      <c r="C14" s="47"/>
+        <v>45751</v>
+      </c>
+      <c r="C14" s="47">
+        <v>1</v>
+      </c>
       <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -2336,18 +2351,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="50">
-        <v>45744</v>
-      </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="36"/>
+        <v>45751</v>
+      </c>
+      <c r="C15" s="51">
+        <v>1</v>
+      </c>
+      <c r="D15" s="52">
+        <v>20</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>36</v>
+      </c>
       <c r="G15" s="56"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -2360,15 +2383,23 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="46"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="46">
+        <v>45751</v>
+      </c>
       <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="48">
+        <v>15</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G16" s="55"/>
       <c r="O16">
         <v>40</v>
@@ -8677,11 +8708,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8689,7 +8720,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8767,7 +8798,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
@@ -8779,7 +8810,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>0.13541666666666666</v>
+        <v>0.17708333333333334</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8789,7 +8820,7 @@
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8797,7 +8828,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8806,7 +8837,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.21180555555555552</v>
+        <v>0.31944444444444448</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9043,6 +9074,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9051,15 +9091,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9082,6 +9113,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9090,12 +9129,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
devlopement du code pour navigation,redirection avec des bouttons, Label plus aproche au figma maquette.  Modiffication des modeles d'application mobile, ajout des labels + export de nouvelle maquette
devlopement du code pour navigation,redirection avec des bouttons, creation des styles :Label les buttons plus aproche au figma maquette.  Modiffication des modeles d'application mobile, ajout des labels + export de nouvelle maquette
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46B6A86-603A-4638-AC02-029D29379C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F412E4E8-3E34-42F9-A065-5153CDE680C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="29625" yWindow="495" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="4830" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>JDT GitHub(Commits + release)</t>
+  </si>
+  <si>
+    <t>… discution avec classe et professeur</t>
+  </si>
+  <si>
+    <t>Modiffication des modeles d'application mobile, ajout des labels + export de nouvelle maquette</t>
+  </si>
+  <si>
+    <t>devlopement du code pour navigation,redirection avec des bouttons, Creation des styles:Label les buttons plus aproche au figma maquette</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1094,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>9.7222222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1094,13 +1103,13 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>6.9444444444444448E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.17708333333333334</c:v>
+                  <c:v>0.18402777777777779</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2015,8 +2024,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2069,7 +2078,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 40 minutes</v>
+        <v>0 jours 9 heurs 9 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2084,15 +2093,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>460</v>
+        <v>550</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2406,45 +2415,69 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="50">
+        <v>45758</v>
+      </c>
       <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
+      <c r="D17" s="52">
+        <v>20</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="G17" s="56"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+    <row r="18" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45758</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1</v>
+      </c>
       <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+      <c r="E18" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45758</v>
+      </c>
       <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
+      <c r="D19" s="52">
+        <v>10</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G19" s="56"/>
       <c r="O19">
         <v>55</v>
@@ -8708,7 +8741,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8720,7 +8753,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>5.5555555555555552E-2</v>
+        <v>9.7222222222222224E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8766,7 +8799,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8774,7 +8807,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>6.9444444444444448E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8802,7 +8835,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8810,7 +8843,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>0.17708333333333334</v>
+        <v>0.18402777777777779</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8837,7 +8870,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.31944444444444448</v>
+        <v>0.38194444444444448</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ImportPage.xaml,TagsPage.xaml,TagsStyle,ImportStyle/(Importation dans App.xaml); JDT
devlopement du code pour navigation,redirection avec des bouttons, Creation des styles:Label les buttons plus aproche au figma maquette. Faire ca pour chaque ecran(Tags,Importation), création des Styles pour Import et Tags. Modification des XAML pour Tags et Import;  JDT
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F412E4E8-3E34-42F9-A065-5153CDE680C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850BCDE3-5A34-4CD6-B176-0AE4D64526B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="4830" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -163,7 +163,10 @@
     <t>Modiffication des modeles d'application mobile, ajout des labels + export de nouvelle maquette</t>
   </si>
   <si>
-    <t>devlopement du code pour navigation,redirection avec des bouttons, Creation des styles:Label les buttons plus aproche au figma maquette</t>
+    <t>devlopement du code pour navigation,redirection avec des bouttons, Creation des styles:Label les buttons plus aproche au figma maquette(main)</t>
+  </si>
+  <si>
+    <t>devlopement du code pour navigation,redirection avec des bouttons, Creation des styles:Label les buttons plus aproche au figma maquette. Faire ca pour chaque ecran(Tags,Importation), création des Styles pour Import et Tags. Modification des XAML pour Tags et Import</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1097,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7222222222222224E-2</c:v>
+                  <c:v>0.1388888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2024,8 +2027,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2078,7 +2081,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 9 minutes</v>
+        <v>0 jours 10 heurs 9 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2093,7 +2096,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2101,7 +2104,7 @@
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>550</v>
+        <v>610</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2483,16 +2486,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+    <row r="20" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
+        <v>15</v>
+      </c>
+      <c r="B20" s="46">
+        <v>45758</v>
+      </c>
+      <c r="C20" s="47">
+        <v>1</v>
+      </c>
       <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="36"/>
+      <c r="E20" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>41</v>
+      </c>
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -8741,7 +8752,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8753,7 +8764,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>9.7222222222222224E-2</v>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8870,7 +8881,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.38194444444444448</v>
+        <v>0.42361111111111116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
rebuilding (styles, images) works✅
le projet n'était pas lançable même après le débogage et la reconstruction de l'ensemble du projet, il ne s'est pas lancé normalement, ce n'est pas de ma faute, mais il y avait des erreurs de compilation
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850BCDE3-5A34-4CD6-B176-0AE4D64526B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6670359-93CE-4914-9D1F-832C6946F2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3210" yWindow="0" windowWidth="24840" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Autre</t>
   </si>
   <si>
-    <t>Nom Prénom</t>
-  </si>
-  <si>
     <t>P_App - 335 - Passion Lecture</t>
   </si>
   <si>
@@ -167,6 +164,15 @@
   </si>
   <si>
     <t>devlopement du code pour navigation,redirection avec des bouttons, Creation des styles:Label les buttons plus aproche au figma maquette. Faire ca pour chaque ecran(Tags,Importation), création des Styles pour Import et Tags. Modification des XAML pour Tags et Import</t>
+  </si>
+  <si>
+    <t>Nademo Yosef</t>
+  </si>
+  <si>
+    <t>debuggin , le projet n'était pas lançable même après le débogage et la reconstruction de l'ensemble du projet, il ne s'est pas lancé normalement, ce n'est pas de ma faute, mais il y avait des erreurs de compilation</t>
+  </si>
+  <si>
+    <t>rebuilding du projet</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1103,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1388888888888889</c:v>
+                  <c:v>0.15972222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2026,9 +2032,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
@@ -2072,7 +2078,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
@@ -2081,7 +2087,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 10 heurs 9 minutes</v>
+        <v>0 jours 10 heurs 40 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2089,7 +2095,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="23.25" hidden="1" x14ac:dyDescent="0.35">
@@ -2100,11 +2106,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>610</v>
+        <v>640</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2123,19 +2129,19 @@
         <v>12</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2154,7 +2160,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="54"/>
     </row>
@@ -2174,7 +2180,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="55"/>
       <c r="M8" t="s">
@@ -2203,7 +2209,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="56"/>
       <c r="M9" t="s">
@@ -2232,7 +2238,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="55"/>
       <c r="M10" t="s">
@@ -2261,7 +2267,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
@@ -2290,7 +2296,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
@@ -2321,7 +2327,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
@@ -2350,7 +2356,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
@@ -2381,7 +2387,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="56"/>
       <c r="M15" t="s">
@@ -2410,7 +2416,7 @@
         <v>22</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="55"/>
       <c r="O16">
@@ -2433,7 +2439,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="56"/>
       <c r="O17">
@@ -2456,7 +2462,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="55"/>
       <c r="O18">
@@ -2479,7 +2485,7 @@
         <v>21</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="56"/>
       <c r="O19">
@@ -2502,21 +2508,31 @@
         <v>4</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" s="55"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
+    <row r="21" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B21" s="50">
+        <v>45779</v>
+      </c>
       <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="56"/>
+      <c r="D21" s="52">
+        <v>30</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
@@ -8756,7 +8772,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8764,7 +8780,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.1388888888888889</v>
+        <v>0.15972222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8881,7 +8897,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.42361111111111116</v>
+        <v>0.44444444444444448</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9118,15 +9134,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9135,6 +9142,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9157,14 +9173,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9173,4 +9181,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
implementation du backend + connexion avec DB + appmobile(en utilisant le guide) + jdt
implementation du backend + connexion avec DB + appmobile(en utilisant le guide) + jdt
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6670359-93CE-4914-9D1F-832C6946F2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3F3FA-6F9A-425C-9C53-9C41A5C21071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="0" windowWidth="24840" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>rebuilding du projet</t>
+  </si>
+  <si>
+    <t>implementation du backend + connexion avec DB + appmobile(en utilisant le guide)</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1106,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15972222222222221</c:v>
+                  <c:v>0.22222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2032,9 +2035,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2090,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 10 heurs 40 minutes</v>
+        <v>0 jours 12 heurs 9 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2102,15 +2105,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>640</v>
+        <v>730</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2535,15 +2538,25 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B22" s="46">
+        <v>45779</v>
+      </c>
+      <c r="C22" s="47">
+        <v>1</v>
+      </c>
+      <c r="D22" s="48">
+        <v>30</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -8768,11 +8781,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8780,7 +8793,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.15972222222222221</v>
+        <v>0.22222222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8897,7 +8910,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.44444444444444448</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Backend(toutes les routes) ;Manual Test Scenarios for EPUB Reader Application
test_scenarios.md
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ED0A1C-F9D5-4691-9369-1144460C0F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F43F64-226A-4F39-B8B1-B643501EBC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="31440" yWindow="435" windowWidth="23520" windowHeight="14235" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="23520" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>insomnia, VS, xaml</t>
+  </si>
+  <si>
+    <t>Backend(toutes les routes)</t>
+  </si>
+  <si>
+    <t>MVVM application des routes dans les ecrans d'application mobile</t>
+  </si>
+  <si>
+    <t>Manual Test Scenarios for EPUB Reader Application</t>
+  </si>
+  <si>
+    <t>test_scenarios.md</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1148,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43055555555555558</c:v>
+                  <c:v>0.51388888888888884</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.0833333333333332E-2</c:v>
@@ -2065,9 +2077,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2120,7 +2132,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 17 heurs 10 minutes</v>
+        <v>0 jours 19 heurs 39 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2135,15 +2147,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>660</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>1030</v>
+        <v>1180</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2700,11 +2712,13 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="46">
+        <v>45793</v>
+      </c>
       <c r="C28" s="47"/>
       <c r="D28" s="48">
         <v>30</v>
@@ -2718,47 +2732,75 @@
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="str">
+      <c r="A29" s="16">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
+        <v>21</v>
+      </c>
+      <c r="B29" s="50">
+        <v>45800</v>
+      </c>
+      <c r="C29" s="51">
+        <v>1</v>
+      </c>
       <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="35"/>
+      <c r="E29" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>55</v>
+      </c>
       <c r="G29" s="56"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="str">
+      <c r="A30" s="8">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="47"/>
+        <v>21</v>
+      </c>
+      <c r="B30" s="46">
+        <v>45800</v>
+      </c>
+      <c r="C30" s="47">
+        <v>1</v>
+      </c>
       <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="36"/>
+      <c r="E30" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>56</v>
+      </c>
       <c r="G30" s="55"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="str">
+      <c r="A31" s="16">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B31" s="50">
+        <v>45800</v>
+      </c>
       <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="56"/>
+      <c r="D31" s="52">
+        <v>30</v>
+      </c>
+      <c r="E31" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="str">
+      <c r="A32" s="8">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B32" s="46">
+        <v>45800</v>
+      </c>
       <c r="C32" s="47"/>
       <c r="D32" s="48"/>
       <c r="E32" s="49"/>
@@ -8867,7 +8909,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8879,7 +8921,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.43055555555555558</v>
+        <v>0.51388888888888884</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8889,7 +8931,7 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C6" s="26" t="str">
         <f>'Journal de travail'!M10</f>
@@ -8897,7 +8939,7 @@
       </c>
       <c r="D6" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -8996,7 +9038,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.71527777777777779</v>
+        <v>0.81944444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9021,6 +9063,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9243,15 +9294,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
@@ -9264,6 +9306,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9280,12 +9330,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
insomnia modification des routes (Export); MVVM application des routes dans les ecrans d'application mobile (Models, ViewModels; Code-behind; debugging; ecrans ALL);;J'ai passé 10 minutes à travailler sur JDT, marqué tous les points de mon proccesus d'Implémentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F43F64-226A-4F39-B8B1-B643501EBC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FD9936-843F-4C38-909B-1001649ADC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="23520" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3960" yWindow="540" windowWidth="23520" windowHeight="14235" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -208,9 +208,6 @@
     <t>insomnia, VS, xaml</t>
   </si>
   <si>
-    <t>Backend(toutes les routes)</t>
-  </si>
-  <si>
     <t>MVVM application des routes dans les ecrans d'application mobile</t>
   </si>
   <si>
@@ -218,6 +215,18 @@
   </si>
   <si>
     <t>test_scenarios.md</t>
+  </si>
+  <si>
+    <t>J'ai passé 10 minutes à travailler sur JDT, marqué tous les points de mon proccesus d'Implémentation</t>
+  </si>
+  <si>
+    <t>Models, ViewModels; Code-behind; debugging; ecrans ALL</t>
+  </si>
+  <si>
+    <t>insomnia</t>
+  </si>
+  <si>
+    <t>Backend(toutes les routes) ; insomnia modification des routes (Export)</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -527,6 +536,17 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1154,7 +1174,7 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6.9444444444444448E-2</c:v>
@@ -2078,8 +2098,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2114,11 +2134,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2132,7 +2152,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 19 heurs 39 minutes</v>
+        <v>0 jours 19 heurs 49 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2151,20 +2171,20 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>1180</v>
+        <v>1190</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="61"/>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
@@ -2747,9 +2767,11 @@
         <v>4</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" s="56"/>
+        <v>61</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
@@ -2767,9 +2789,11 @@
         <v>4</v>
       </c>
       <c r="F30" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="55"/>
+        <v>55</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
@@ -2787,10 +2811,10 @@
         <v>5</v>
       </c>
       <c r="F31" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="56" t="s">
         <v>57</v>
-      </c>
-      <c r="G31" s="56" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2802,9 +2826,15 @@
         <v>45800</v>
       </c>
       <c r="C32" s="47"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="36"/>
+      <c r="D32" s="52">
+        <v>10</v>
+      </c>
+      <c r="E32" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,9 +2844,9 @@
       </c>
       <c r="B33" s="50"/>
       <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="35"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="56"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -8813,7 +8843,7 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7:E532">
+  <conditionalFormatting sqref="E34:E532 E7:E32">
     <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
@@ -8843,10 +8873,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D34:D532 D7:D32" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
       <formula1>$O$7:$O$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E532" xr:uid="{5717AF9A-5C26-4256-9473-8948342ED6D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E34:E532 E7:E32" xr:uid="{5717AF9A-5C26-4256-9473-8948342ED6D3}">
       <formula1>$M$7:$M$15</formula1>
     </dataValidation>
   </dataValidations>
@@ -8949,7 +8979,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8957,7 +8987,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9038,7 +9068,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.81944444444444442</v>
+        <v>0.82638888888888884</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ReadnigPage(UI,apiPaths,buttons,lecture); Import Service;JDT GitHub(Commits + release); tests manuel; load more ; libraripage-viewmodel-.xaml.cs; readpage-viewmodel-.xaml.cs; model
add a numericid; tests manuel ;4h
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdjdj\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE6E718-C78F-41A2-8622-875AD8333931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39EAD2-9637-424F-A671-D649C4535416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="540" windowWidth="23520" windowHeight="14235" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -231,6 +231,54 @@
   <si>
     <t>docker script SQL</t>
   </si>
+  <si>
+    <t>MAUI MVVM</t>
+  </si>
+  <si>
+    <t>configuration service that will handle the API endpoint configuration; A…
+…piConfiguration.cs ; ApiPage.xaml; tags works✅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you're developing/testing on an Android emulator:
+10.0.2.2 is a special IP address that Android emulator uses to connect to your computer's localhost
+So when your app runs in the emulator and tries to reach 10.0.2.2:3000, it actually connects to localhost:3000 on your development machine where Docker is runnings
+</t>
+  </si>
+  <si>
+    <t>ApiPageVM; triage par tags; triage par dates ;tags xaml ; tags model; li…
+…braryPage.xaml ;libraryPageVM;  BooksModel.cs;  HttpClient</t>
+  </si>
+  <si>
+    <t>librarypage, filter(year, tags), research, importpage; readPage; api
+readpage[inprgress]</t>
+  </si>
+  <si>
+    <t>Instructions ! Update README.md</t>
+  </si>
+  <si>
+    <t>ReadPage; ReadPageViewModel; LibraryPage ; app.js(image cover)
+required adm-zip package for handling EPUB files:
+ npm install adm-zip</t>
+  </si>
+  <si>
+    <t>Insomnia</t>
+  </si>
+  <si>
+    <t>general routes</t>
+  </si>
+  <si>
+    <t>api(BLOB✅ corrected); ApiService(right path and debuuging + console.log)…
+…; Covers ✅</t>
+  </si>
+  <si>
+    <t>ReadnigPage(UI,apiPaths,buttons,lecture)</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tests manuel</t>
+  </si>
 </sst>
 </file>
 
@@ -413,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -542,17 +590,6 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -565,6 +602,80 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -737,80 +848,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -833,7 +870,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -900,7 +937,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1171,13 +1208,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53472222222222221</c:v>
+                  <c:v>1.0486111111111112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7777777777777776E-2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6.9444444444444448E-2</c:v>
@@ -1895,18 +1932,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2101,11 +2138,11 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+      <pane ySplit="6" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.625" style="8" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
@@ -2137,11 +2174,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2155,7 +2192,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 20 heurs 19 minutes</v>
+        <v>1 jours 9 heurs 39 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2170,24 +2207,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>660</v>
+        <v>1380</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>560</v>
+        <v>640</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>1220</v>
+        <v>2020</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
@@ -2847,9 +2884,9 @@
       </c>
       <c r="B33" s="50"/>
       <c r="C33" s="51"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="59"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="55"/>
       <c r="G33" s="56"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2873,147 +2910,245 @@
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="str">
+      <c r="A35" s="16">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="51"/>
+        <v>22</v>
+      </c>
+      <c r="B35" s="50">
+        <v>45805</v>
+      </c>
+      <c r="C35" s="51">
+        <v>1</v>
+      </c>
       <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>63</v>
+      </c>
       <c r="G35" s="56"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="str">
+    <row r="36" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="46"/>
-      <c r="C36" s="47"/>
+        <v>22</v>
+      </c>
+      <c r="B36" s="46">
+        <v>45806</v>
+      </c>
+      <c r="C36" s="47">
+        <v>2</v>
+      </c>
       <c r="D36" s="48"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="55"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="str">
+      <c r="E36" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="16">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
+        <v>22</v>
+      </c>
+      <c r="B37" s="50">
+        <v>45806</v>
+      </c>
+      <c r="C37" s="51">
+        <v>2</v>
+      </c>
       <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>66</v>
+      </c>
       <c r="G37" s="56"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="str">
+    <row r="38" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
-        <v/>
-      </c>
-      <c r="B38" s="46"/>
-      <c r="C38" s="47"/>
+        <v>22</v>
+      </c>
+      <c r="B38" s="46">
+        <v>45806</v>
+      </c>
+      <c r="C38" s="47">
+        <v>2</v>
+      </c>
       <c r="D38" s="48"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="35"/>
+      <c r="E38" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>67</v>
+      </c>
       <c r="G38" s="55"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="str">
+      <c r="A39" s="16">
         <f>IF(ISBLANK(B39),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B39))</f>
-        <v/>
-      </c>
-      <c r="B39" s="50"/>
+        <v>22</v>
+      </c>
+      <c r="B39" s="50">
+        <v>45808</v>
+      </c>
       <c r="C39" s="51"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="35"/>
+      <c r="D39" s="52">
+        <v>10</v>
+      </c>
+      <c r="E39" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="G39" s="56"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="str">
+    <row r="40" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="B40" s="46">
+        <v>45808</v>
+      </c>
       <c r="C40" s="47"/>
       <c r="D40" s="48"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="35"/>
+      <c r="E40" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>69</v>
+      </c>
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="str">
+      <c r="A41" s="16">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="50"/>
+        <v>22</v>
+      </c>
+      <c r="B41" s="50">
+        <v>45808</v>
+      </c>
       <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="56"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="str">
+      <c r="D41" s="52">
+        <v>20</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" s="56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="47"/>
+        <v>22</v>
+      </c>
+      <c r="B42" s="46">
+        <v>45808</v>
+      </c>
+      <c r="C42" s="47">
+        <v>2</v>
+      </c>
       <c r="D42" s="48"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="35"/>
+      <c r="E42" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>72</v>
+      </c>
       <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="str">
+      <c r="A43" s="16">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
+        <v>22</v>
+      </c>
+      <c r="B43" s="50">
+        <v>45808</v>
+      </c>
+      <c r="C43" s="51">
+        <v>2</v>
+      </c>
       <c r="D43" s="52"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="35"/>
+      <c r="E43" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>73</v>
+      </c>
       <c r="G43" s="56"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="str">
+      <c r="A44" s="8">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="46"/>
-      <c r="C44" s="47"/>
+        <v>22</v>
+      </c>
+      <c r="B44" s="46">
+        <v>45808</v>
+      </c>
+      <c r="C44" s="47">
+        <v>1</v>
+      </c>
       <c r="D44" s="48"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="35"/>
+      <c r="E44" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="G44" s="55"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="str">
+      <c r="A45" s="16">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="50"/>
+        <v>22</v>
+      </c>
+      <c r="B45" s="50">
+        <v>45808</v>
+      </c>
       <c r="C45" s="51"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="35"/>
+      <c r="D45" s="52">
+        <v>25</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="G45" s="56"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="str">
+      <c r="A46" s="8">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="B46" s="46">
+        <v>45808</v>
+      </c>
       <c r="C46" s="47"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="35"/>
+      <c r="D46" s="48">
+        <v>25</v>
+      </c>
+      <c r="E46" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>36</v>
+      </c>
       <c r="G46" s="55"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -8854,29 +8989,29 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E34:E532 E7:E32">
-    <cfRule type="expression" dxfId="16" priority="1">
+  <conditionalFormatting sqref="E7:E32 E34:E532">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8908,7 +9043,7 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="10.875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="29" bestFit="1" customWidth="1"/>
@@ -8950,11 +9085,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>420</v>
+        <v>1140</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8962,7 +9097,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.53472222222222221</v>
+        <v>1.0486111111111112</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8972,7 +9107,7 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C6" s="26" t="str">
         <f>'Journal de travail'!M10</f>
@@ -8980,7 +9115,7 @@
       </c>
       <c r="D6" s="33">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -8990,7 +9125,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8998,7 +9133,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>2.7777777777777776E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9079,7 +9214,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.84722222222222221</v>
+        <v>1.4027777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9093,14 +9228,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9327,21 +9460,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9366,9 +9498,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
BookTagsPage; BookTagsViewModel; TagItemViewModel; ApiService; LibraryPageViewModel; Insomnia; assosiation between books and tags; video
/books/:id/tags   API
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_NademoYosef.xlsx
+++ b/Documentation/Journal-de-Travail_NademoYosef.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdjdj\Documents\GitHub\Passion_lecture_Mobile\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39EAD2-9637-424F-A671-D649C4535416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ABB677-2DF0-450F-941B-3F35FF4FA7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t xml:space="preserve"> tests manuel</t>
+  </si>
+  <si>
+    <t>BookTagsPage; BookTagsViewModel; TagItemViewModel; ApiService; LibraryPageViewModel; Insomnia; assosiation between books and tags</t>
   </si>
 </sst>
 </file>
@@ -1208,13 +1211,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0486111111111112</c:v>
+                  <c:v>1.1736111111111112</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>7.9861111111111105E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6.9444444444444448E-2</c:v>
@@ -2139,7 +2142,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2195,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>1 jours 9 heurs 39 minutes</v>
+        <v>1 jours 13 heurs 4 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2207,15 +2210,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>1380</v>
+        <v>1560</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>640</v>
+        <v>665</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>2020</v>
+        <v>2225</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -3152,27 +3155,43 @@
       <c r="G46" s="55"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="str">
+      <c r="A47" s="16">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="50"/>
-      <c r="C47" s="51"/>
+        <v>22</v>
+      </c>
+      <c r="B47" s="50">
+        <v>45809</v>
+      </c>
+      <c r="C47" s="51">
+        <v>3</v>
+      </c>
       <c r="D47" s="52"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="35"/>
+      <c r="E47" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>76</v>
+      </c>
       <c r="G47" s="56"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="str">
+      <c r="A48" s="8">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v/>
-      </c>
-      <c r="B48" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="B48" s="46">
+        <v>45809</v>
+      </c>
       <c r="C48" s="47"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="35"/>
+      <c r="D48" s="48">
+        <v>25</v>
+      </c>
+      <c r="E48" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="35" t="s">
+        <v>36</v>
+      </c>
       <c r="G48" s="55"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -9085,7 +9104,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>1140</v>
+        <v>1320</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -9097,7 +9116,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>1.0486111111111112</v>
+        <v>1.1736111111111112</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9125,7 +9144,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -9133,7 +9152,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>7.9861111111111105E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9214,7 +9233,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>1.4027777777777779</v>
+        <v>1.5451388888888891</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9228,12 +9247,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9460,20 +9481,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9498,12 +9520,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>